<commit_message>
palavra chave e pegando numeros com virgula
</commit_message>
<xml_diff>
--- a/palavras_chave.xlsx
+++ b/palavras_chave.xlsx
@@ -2,21 +2,46 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>times</t>
+  </si>
+  <si>
+    <t>flu</t>
+  </si>
+  <si>
+    <t>vasco</t>
+  </si>
+  <si>
+    <t>fla</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,18 +65,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -130,7 +173,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -165,7 +207,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -342,12 +383,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
palavra chave ainda não terminado, construcao de tabela
</commit_message>
<xml_diff>
--- a/palavras_chave.xlsx
+++ b/palavras_chave.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>times</t>
+    <t>palavra</t>
   </si>
   <si>
-    <t>flu</t>
+    <t>correspondentes</t>
   </si>
   <si>
-    <t>vasco</t>
+    <t>lucrou</t>
   </si>
   <si>
-    <t>fla</t>
+    <t>Game</t>
   </si>
 </sst>
 </file>
@@ -383,39 +383,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
         <v>3</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
interface, mudanca em local, captura de numeros e palavras criacao de planilha
</commit_message>
<xml_diff>
--- a/palavras_chave.xlsx
+++ b/palavras_chave.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>palavra</t>
   </si>
@@ -25,7 +25,13 @@
     <t>lucrou</t>
   </si>
   <si>
-    <t>Game</t>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2020.</t>
   </si>
 </sst>
 </file>
@@ -404,8 +410,8 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -415,8 +421,8 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alterando valores de strings para inteiros e floats
</commit_message>
<xml_diff>
--- a/palavras_chave.xlsx
+++ b/palavras_chave.xlsx
@@ -14,24 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>palavra</t>
+    <t>Dados</t>
+  </si>
+  <si>
+    <t>numeros</t>
   </si>
   <si>
     <t>correspondentes</t>
-  </si>
-  <si>
-    <t>lucrou</t>
-  </si>
-  <si>
-    <t>Games</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2020.</t>
   </si>
 </sst>
 </file>
@@ -389,40 +380,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>34</v>
+      </c>
+      <c r="D3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
         <v>5</v>
+      </c>
+      <c r="C7">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>61</v>
+      </c>
+      <c r="D9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>55</v>
+      </c>
+      <c r="D16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>32</v>
+      </c>
+      <c r="D23">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>74</v>
+      </c>
+      <c r="D25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>16</v>
+      </c>
+      <c r="D29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>61</v>
+      </c>
+      <c r="D32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>55</v>
+      </c>
+      <c r="D33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>51</v>
+      </c>
+      <c r="D34">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>